<commit_message>
added web dev code
</commit_message>
<xml_diff>
--- a/Python/readingexcel/project-data.xlsx
+++ b/Python/readingexcel/project-data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ish\OneDrive - Carleton University\work details\Projects\Self assessment 4th year project\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ish\Desktop\small projects\Small_Project_Code\Python\readingexcel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="11_990AAE22D25631ED5E38DBBD46CC2A17CC548F29" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{98223731-BD66-438A-B32F-A2D868898007}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64A84428-893B-4511-BCA7-1796CA0745AA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3480" yWindow="405" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Project List" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>Labiche</t>
   </si>
@@ -33,30 +33,6 @@
     <t>Singh</t>
   </si>
   <si>
-    <t>First name</t>
-  </si>
-  <si>
-    <t>Last name</t>
-  </si>
-  <si>
-    <t>ID Number</t>
-  </si>
-  <si>
-    <t>Title</t>
-  </si>
-  <si>
-    <t>Student</t>
-  </si>
-  <si>
-    <t>Co-supervisor</t>
-  </si>
-  <si>
-    <t>Supervisor</t>
-  </si>
-  <si>
-    <t>Group</t>
-  </si>
-  <si>
     <t>Crowd-source grocery store layouts for dynamically sorted shopping lists</t>
   </si>
   <si>
@@ -93,7 +69,28 @@
     <t>Ishdeep</t>
   </si>
   <si>
-    <t>Group No</t>
+    <t>groupNo</t>
+  </si>
+  <si>
+    <t>title</t>
+  </si>
+  <si>
+    <t>supervisor</t>
+  </si>
+  <si>
+    <t>coSupervisor</t>
+  </si>
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>lastName</t>
+  </si>
+  <si>
+    <t>firstName</t>
+  </si>
+  <si>
+    <t>AssessmentStatus</t>
   </si>
 </sst>
 </file>
@@ -225,7 +222,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFill="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
@@ -245,10 +242,13 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -535,10 +535,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G9"/>
+  <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -553,154 +553,155 @@
     <col min="8" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="14" t="s">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="F1" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="G1" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="H1" s="14" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="16">
+        <v>52</v>
+      </c>
+      <c r="B2" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="17"/>
+      <c r="E2" s="9">
+        <v>1</v>
+      </c>
+      <c r="F2" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="G2" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="H2" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="16"/>
+      <c r="B3" s="17"/>
+      <c r="C3" s="17"/>
+      <c r="D3" s="17"/>
+      <c r="E3" s="9">
+        <v>2</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="H3" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="16"/>
+      <c r="B4" s="17"/>
+      <c r="C4" s="17"/>
+      <c r="D4" s="17"/>
+      <c r="E4" s="1">
+        <v>3</v>
+      </c>
+      <c r="F4" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="14"/>
-      <c r="C1" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="D1" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="E1" s="14" t="s">
-        <v>6</v>
-      </c>
-      <c r="F1" s="14"/>
-      <c r="G1" s="14"/>
+      <c r="G4" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="H4" s="1">
+        <v>0</v>
+      </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="B2" s="10" t="s">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="16">
+        <v>27</v>
+      </c>
+      <c r="B5" s="17" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="D5" s="17"/>
+      <c r="E5" s="7">
+        <v>4</v>
+      </c>
+      <c r="F5" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="G5" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="H5" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="16"/>
+      <c r="B6" s="17"/>
+      <c r="C6" s="17"/>
+      <c r="D6" s="17"/>
+      <c r="E6" s="12">
         <v>5</v>
       </c>
-      <c r="C2" s="14"/>
-      <c r="D2" s="14"/>
-      <c r="E2" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="F2" s="10" t="s">
-        <v>3</v>
-      </c>
-      <c r="G2" s="10" t="s">
-        <v>2</v>
+      <c r="F6" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="H6" s="1">
+        <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="15">
-        <v>52</v>
-      </c>
-      <c r="B3" s="16" t="s">
-        <v>10</v>
-      </c>
-      <c r="C3" s="16" t="s">
-        <v>12</v>
-      </c>
-      <c r="D3" s="16"/>
-      <c r="E3" s="9">
-        <v>1</v>
-      </c>
-      <c r="F3" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="G3" s="8" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="15"/>
-      <c r="B4" s="16"/>
-      <c r="C4" s="16"/>
-      <c r="D4" s="16"/>
-      <c r="E4" s="9">
-        <v>2</v>
-      </c>
-      <c r="F4" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="G4" s="5" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="15"/>
-      <c r="B5" s="16"/>
-      <c r="C5" s="16"/>
-      <c r="D5" s="16"/>
-      <c r="E5" s="1">
-        <v>3</v>
-      </c>
-      <c r="F5" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="G5" s="5" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="15">
-        <v>27</v>
-      </c>
-      <c r="B6" s="16" t="s">
-        <v>11</v>
-      </c>
-      <c r="C6" s="16" t="s">
-        <v>0</v>
-      </c>
-      <c r="D6" s="16"/>
-      <c r="E6" s="7">
-        <v>4</v>
-      </c>
-      <c r="F6" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="G6" s="6" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="15"/>
-      <c r="B7" s="16"/>
-      <c r="C7" s="16"/>
-      <c r="D7" s="16"/>
-      <c r="E7" s="12">
-        <v>5</v>
-      </c>
-      <c r="F7" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="G7" s="4" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="13"/>
-      <c r="B9" s="13"/>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
-      <c r="F9" s="3"/>
-      <c r="G9" s="3"/>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="15"/>
+      <c r="B8" s="15"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="3"/>
     </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
-  <mergeCells count="13">
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="D1:D2"/>
-    <mergeCell ref="E1:G1"/>
-    <mergeCell ref="A3:A5"/>
-    <mergeCell ref="B3:B5"/>
-    <mergeCell ref="C3:C5"/>
-    <mergeCell ref="D3:D5"/>
-    <mergeCell ref="A6:A7"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="C6:C7"/>
-    <mergeCell ref="D6:D7"/>
+  <mergeCells count="9">
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="A2:A4"/>
+    <mergeCell ref="B2:B4"/>
+    <mergeCell ref="C2:C4"/>
+    <mergeCell ref="D2:D4"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="D5:D6"/>
   </mergeCells>
   <pageMargins left="0.1" right="0.1" top="0.1" bottom="0.1" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape" r:id="rId1"/>

</xml_diff>